<commit_message>
Update generate_one_sample_t_test_wtp.py, generate_one_sample_t_test_wtp_HealthyVsUnhealthy.py, and 91 more files...
</commit_message>
<xml_diff>
--- a/fMRI/fx/models/WTP/fx_conditions_allwaves_contrast_design_all.xlsx
+++ b/fMRI/fx/models/WTP/fx_conditions_allwaves_contrast_design_all.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/denicia/DEV/DEV_scripts/fMRI/fx/models/WTP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C196D4-0095-BF48-BF0E-B4E0A5774B53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1487CF04-6F7E-1545-9E12-C0FC9394703E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2540" yWindow="540" windowWidth="40360" windowHeight="22540" xr2:uid="{C2E55B3A-6737-DF4B-B7A9-D1BA84A8D149}"/>
+    <workbookView xWindow="3060" yWindow="500" windowWidth="40360" windowHeight="22540" xr2:uid="{C2E55B3A-6737-DF4B-B7A9-D1BA84A8D149}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -936,10 +936,10 @@
   <dimension ref="A1:AE81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="Z2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="V63" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G79" sqref="G79"/>
+      <selection pane="bottomRight" activeCell="W81" sqref="W81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9511,7 +9511,7 @@
         <v>0</v>
       </c>
       <c r="Q81" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f>Q80&amp;" "&amp;P81</f>
         <v>0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0</v>
       </c>
       <c r="R81" s="1">

</xml_diff>